<commit_message>
backtestimg funcionando, no cgoia el pais
</commit_message>
<xml_diff>
--- a/Futbol.xlsx
+++ b/Futbol.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K68"/>
+  <dimension ref="A1:K62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,11 +496,11 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45024</v>
+        <v>45052</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Primera División</t>
+          <t>Copa del Rey</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -510,12 +510,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Villarreal</t>
+          <t>Osasuna</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2-3</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -525,27 +525,27 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>29.37</v>
+        <v>31.97</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45028</v>
+        <v>45055</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -559,42 +559,42 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Chelsea</t>
+          <t>Manchester City</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2-0</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>29.92</v>
+        <v>31.99</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45031</v>
+        <v>45059</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -603,31 +603,31 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Cádiz</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Getafe</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0-2</t>
+          <t>1-0</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="H4" t="n">
-        <v>30.85</v>
+        <v>30.76</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -643,7 +643,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45034</v>
+        <v>45063</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -652,7 +652,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Chelsea</t>
+          <t>Manchester City</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -662,37 +662,39 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0-2</t>
+          <t>4-0</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="H5" t="n">
-        <v>31.08</v>
+        <v>30.99</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Perdido</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr"/>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>-1.158824735315502</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45038</v>
+        <v>45067</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -701,22 +703,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Valencia</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Celta</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2-0</t>
+          <t>1-0</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -725,23 +727,23 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>31.82</v>
+        <v>31.49</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Perdido</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45041</v>
+        <v>45070</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -750,49 +752,47 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Girona</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Rayo Vallecano</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>4-2</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>31.37</v>
+        <v>30.82</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K7" t="n">
-        <v>1.512675769914667</v>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45045</v>
+        <v>45073</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -801,22 +801,22 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Sevilla</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Almería</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>4-2</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -825,7 +825,7 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>31.06</v>
+        <v>31.18</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -841,7 +841,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45048</v>
+        <v>45081</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -850,53 +850,51 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Real Sociedad</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Athletic</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2-0</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>31.06</v>
+        <v>31.4</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
+          <t>NO SE REALIZA OPERACION</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45052</v>
+        <v>45131</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Copa del Rey</t>
+          <t>Soccer Champions Tour</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -906,26 +904,26 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Osasuna</t>
+          <t>Milan</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2-1</t>
+          <t>3-2</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="H10" t="n">
-        <v>31.97</v>
+        <v>30.45</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -941,11 +939,11 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45055</v>
+        <v>45134</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Champions League</t>
+          <t>Soccer Champions Tour</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -955,66 +953,66 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Manchester City</t>
+          <t>Manchester United</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>2-0</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>31.99</v>
+        <v>31.84</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45059</v>
+        <v>45136</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Primera División</t>
+          <t>Soccer Champions Tour</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Barcelona</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Getafe</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>3-0</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1023,32 +1021,34 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>30.76</v>
+        <v>31.79</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Perdido</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr"/>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
+        <v>2.336827719614369</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45063</v>
+        <v>45141</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Champions League</t>
+          <t>Soccer Champions Tour</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Manchester City</t>
+          <t>Juventus</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1058,21 +1058,21 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>4-0</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>30.99</v>
+        <v>31.15</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -1081,16 +1081,14 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K13" t="n">
-        <v>-1.158824735315502</v>
-      </c>
+          <t>NO SE REALIZA OPERACION</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45067</v>
+        <v>45150</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1099,7 +1097,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Valencia</t>
+          <t>Athletic</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1109,37 +1107,37 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>0-2</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>31.49</v>
+        <v>31.68</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45070</v>
+        <v>45157</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1148,31 +1146,31 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Almería</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Rayo Vallecano</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2-1</t>
+          <t>1-3</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>30.82</v>
+        <v>31.31</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -1188,7 +1186,7 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45073</v>
+        <v>45163</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1197,7 +1195,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Sevilla</t>
+          <t>Celta</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1207,21 +1205,21 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1-2</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>31.18</v>
+        <v>31.67</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1237,7 +1235,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45081</v>
+        <v>45171</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1251,17 +1249,17 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Athletic</t>
+          <t>Getafe</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1270,27 +1268,27 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>31.4</v>
+        <v>32.37</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45131</v>
+        <v>45186</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Soccer Champions Tour</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1300,26 +1298,26 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Milan</t>
+          <t>Real Sociedad</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>3-2</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>30.45</v>
+        <v>33.62</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -1335,11 +1333,11 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45134</v>
+        <v>45189</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Soccer Champions Tour</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1349,17 +1347,17 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Manchester United</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2-0</t>
+          <t>1-0</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1368,7 +1366,7 @@
         </is>
       </c>
       <c r="H19" t="n">
-        <v>31.84</v>
+        <v>34.36</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -1384,16 +1382,16 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45136</v>
+        <v>45193</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Soccer Champions Tour</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Barcelona</t>
+          <t>Atlético</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1403,7 +1401,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>3-0</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1413,11 +1411,11 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H20" t="n">
-        <v>31.79</v>
+        <v>33.83</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -1430,61 +1428,61 @@
         </is>
       </c>
       <c r="K20" t="n">
-        <v>2.336827719614369</v>
+        <v>4.207997278439312</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45141</v>
+        <v>45196</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Soccer Champions Tour</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Juventus</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Las Palmas</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>2-0</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>31.15</v>
+        <v>33.8</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45150</v>
+        <v>45199</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1493,7 +1491,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Athletic</t>
+          <t>Girona</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1503,7 +1501,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0-2</t>
+          <t>0-3</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1513,11 +1511,11 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>31.68</v>
+        <v>33.72</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
@@ -1533,16 +1531,16 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45157</v>
+        <v>45202</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Primera División</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Almería</t>
+          <t>Napoli</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1552,12 +1550,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1-3</t>
+          <t>2-3</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1566,7 +1564,7 @@
         </is>
       </c>
       <c r="H23" t="n">
-        <v>31.31</v>
+        <v>33.45</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -1582,7 +1580,7 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45163</v>
+        <v>45206</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1591,31 +1589,31 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Celta</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Osasuna</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>4-0</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="H24" t="n">
-        <v>31.67</v>
+        <v>32.89</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -1631,7 +1629,7 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45171</v>
+        <v>45220</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1640,22 +1638,22 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Sevilla</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Getafe</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2-1</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1664,56 +1662,56 @@
         </is>
       </c>
       <c r="H25" t="n">
-        <v>32.37</v>
+        <v>32.41</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45186</v>
+        <v>45223</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Primera División</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Sporting Braga</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Real Sociedad</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2-1</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="H26" t="n">
-        <v>33.62</v>
+        <v>32.62</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
@@ -1729,26 +1727,26 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45189</v>
+        <v>45227</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Champions League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Barcelona</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Union Berlin</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1758,11 +1756,11 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>34.36</v>
+        <v>33.74</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
@@ -1778,7 +1776,7 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45193</v>
+        <v>45235</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1787,53 +1785,51 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Atlético</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Rayo Vallecano</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>0-0</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H28" t="n">
-        <v>33.83</v>
+        <v>33.5</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K28" t="n">
-        <v>4.207997278439312</v>
-      </c>
+          <t>NO SE REALIZA OPERACION</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45196</v>
+        <v>45238</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Primera División</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1843,17 +1839,17 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Las Palmas</t>
+          <t>Sporting Braga</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2-0</t>
+          <t>3-0</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1862,7 +1858,7 @@
         </is>
       </c>
       <c r="H29" t="n">
-        <v>33.8</v>
+        <v>33.26</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
@@ -1878,7 +1874,7 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45199</v>
+        <v>45241</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1887,31 +1883,31 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Girona</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Valencia</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0-3</t>
+          <t>5-1</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H30" t="n">
-        <v>33.72</v>
+        <v>33.78</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
@@ -1927,16 +1923,16 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45202</v>
+        <v>45256</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Champions League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Napoli</t>
+          <t>Cádiz</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1946,12 +1942,12 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2-3</t>
+          <t>0-3</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1960,7 +1956,7 @@
         </is>
       </c>
       <c r="H31" t="n">
-        <v>33.45</v>
+        <v>36.41</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
@@ -1976,11 +1972,11 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45206</v>
+        <v>45259</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Primera División</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1990,12 +1986,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Osasuna</t>
+          <t>Napoli</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>4-0</t>
+          <t>4-2</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2005,11 +2001,11 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>32.89</v>
+        <v>36.76</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
@@ -2025,7 +2021,7 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45220</v>
+        <v>45262</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -2034,35 +2030,35 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Sevilla</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Granada</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>2-0</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>32.41</v>
+        <v>36.93</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -2074,16 +2070,16 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45223</v>
+        <v>45269</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Champions League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Sporting Braga</t>
+          <t>Real Betis</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2093,7 +2089,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1-2</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2103,36 +2099,36 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>32.62</v>
+        <v>37.46</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45227</v>
+        <v>45272</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Primera División</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Barcelona</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -2142,21 +2138,21 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1-2</t>
+          <t>2-3</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H35" t="n">
-        <v>33.74</v>
+        <v>37.98</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
@@ -2165,14 +2161,14 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45235</v>
+        <v>45277</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -2186,30 +2182,30 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Rayo Vallecano</t>
+          <t>Villarreal</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0-0</t>
+          <t>4-1</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H36" t="n">
-        <v>33.5</v>
+        <v>39.3</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -2221,40 +2217,40 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45238</v>
+        <v>45281</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Champions League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Deportivo Alavés</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Sporting Braga</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>3-0</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H37" t="n">
-        <v>33.26</v>
+        <v>39.77</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
@@ -2263,14 +2259,14 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>45241</v>
+        <v>45294</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -2284,26 +2280,26 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Valencia</t>
+          <t>Mallorca</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>5-1</t>
+          <t>1-0</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H38" t="n">
-        <v>33.78</v>
+        <v>39.41</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
@@ -2312,23 +2308,23 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>45256</v>
+        <v>45297</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Primera División</t>
+          <t>Copa del Rey</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Cádiz</t>
+          <t>Arandina</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -2338,12 +2334,12 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>0-3</t>
+          <t>1-3</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -2352,7 +2348,7 @@
         </is>
       </c>
       <c r="H39" t="n">
-        <v>36.41</v>
+        <v>39.98</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
@@ -2361,18 +2357,18 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45259</v>
+        <v>45301</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Champions League</t>
+          <t>Supercopa de España</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2382,26 +2378,26 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Napoli</t>
+          <t>Atlético</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>4-2</t>
+          <t>5-3</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H40" t="n">
-        <v>36.76</v>
+        <v>38.977</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
@@ -2410,18 +2406,18 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>45262</v>
+        <v>45305</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Primera División</t>
+          <t>Supercopa de España</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2431,26 +2427,26 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Granada</t>
+          <t>Barcelona</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2-0</t>
+          <t>4-1</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H41" t="n">
-        <v>36.93</v>
+        <v>39.797</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
@@ -2466,16 +2462,16 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>45269</v>
+        <v>45309</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Primera División</t>
+          <t>Copa del Rey</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Real Betis</t>
+          <t>Atlético</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -2485,70 +2481,72 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>4-2</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H42" t="n">
-        <v>37.46</v>
+        <v>39.214</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Perdido</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr"/>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="K42" t="n">
+        <v>15.35735694237965</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>45272</v>
+        <v>45312</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Champions League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Union Berlin</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Almería</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2-3</t>
+          <t>3-2</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
       <c r="H43" t="n">
-        <v>37.98</v>
+        <v>39.75</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
@@ -2557,14 +2555,14 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>45277</v>
+        <v>45318</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -2573,31 +2571,31 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Las Palmas</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Villarreal</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>4-1</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H44" t="n">
-        <v>39.3</v>
+        <v>35.66</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
@@ -2606,14 +2604,14 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>45281</v>
+        <v>45323</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -2622,7 +2620,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Deportivo Alavés</t>
+          <t>Getafe</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -2632,7 +2630,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>0-2</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2642,11 +2640,11 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H45" t="n">
-        <v>39.77</v>
+        <v>36.61</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
@@ -2655,14 +2653,14 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>45294</v>
+        <v>45326</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -2676,12 +2674,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Mallorca</t>
+          <t>Atlético</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2691,15 +2689,15 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H46" t="n">
-        <v>39.41</v>
+        <v>36.46</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
@@ -2711,40 +2709,40 @@
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>45297</v>
+        <v>45332</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Copa del Rey</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Arandina</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Girona</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1-3</t>
+          <t>4-0</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H47" t="n">
-        <v>39.98</v>
+        <v>36.21</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
@@ -2753,47 +2751,47 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>45301</v>
+        <v>45335</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Supercopa de España</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Atlético</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>5-3</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H48" t="n">
-        <v>38.977</v>
+        <v>36.39</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
@@ -2802,38 +2800,38 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>45305</v>
+        <v>45340</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Supercopa de España</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Rayo Vallecano</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Barcelona</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>4-1</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -2842,11 +2840,11 @@
         </is>
       </c>
       <c r="H49" t="n">
-        <v>39.797</v>
+        <v>36.45</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -2858,58 +2856,56 @@
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>45309</v>
+        <v>45347</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Copa del Rey</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Atlético</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Sevilla</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>4-2</t>
+          <t>1-0</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H50" t="n">
-        <v>39.214</v>
+        <v>36.94</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K50" t="n">
-        <v>15.35735694237965</v>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>45312</v>
+        <v>45353</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -2918,22 +2914,22 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Valencia</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Almería</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>3-2</t>
+          <t>2-2</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -2942,42 +2938,42 @@
         </is>
       </c>
       <c r="H51" t="n">
-        <v>39.75</v>
+        <v>37.74</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>45318</v>
+        <v>45357</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Primera División</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Las Palmas</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1-2</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -2987,27 +2983,27 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H52" t="n">
-        <v>35.66</v>
+        <v>38.5</v>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>45323</v>
+        <v>45361</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -3016,31 +3012,31 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Getafe</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Celta</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>0-2</t>
+          <t>4-0</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="H53" t="n">
-        <v>36.61</v>
+        <v>38.77</v>
       </c>
       <c r="I53" t="inlineStr">
         <is>
@@ -3056,7 +3052,7 @@
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>45326</v>
+        <v>45367</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -3065,47 +3061,47 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Osasuna</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Atlético</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>2-4</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H54" t="n">
-        <v>36.46</v>
+        <v>40.14</v>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>45332</v>
+        <v>45382</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -3119,17 +3115,17 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Girona</t>
+          <t>Athletic</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>4-0</t>
+          <t>2-0</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -3138,7 +3134,7 @@
         </is>
       </c>
       <c r="H55" t="n">
-        <v>36.21</v>
+        <v>38.48</v>
       </c>
       <c r="I55" t="inlineStr">
         <is>
@@ -3154,7 +3150,7 @@
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>45335</v>
+        <v>45391</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -3163,47 +3159,47 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Manchester City</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>3-3</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H56" t="n">
-        <v>36.39</v>
+        <v>37.78</v>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>45340</v>
+        <v>45395</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -3212,7 +3208,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Rayo Vallecano</t>
+          <t>Mallorca</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -3222,12 +3218,12 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -3236,56 +3232,56 @@
         </is>
       </c>
       <c r="H57" t="n">
-        <v>36.45</v>
+        <v>37.64</v>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>45347</v>
+        <v>45399</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Primera División</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Manchester City</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Sevilla</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>1 (3-4) 1</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H58" t="n">
-        <v>36.94</v>
+        <v>38.66</v>
       </c>
       <c r="I58" t="inlineStr">
         <is>
@@ -3294,14 +3290,14 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>45353</v>
+        <v>45403</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -3310,35 +3306,35 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Valencia</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Barcelona</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2-2</t>
+          <t>3-2</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="H59" t="n">
-        <v>37.74</v>
+        <v>38.46</v>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
@@ -3350,31 +3346,31 @@
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>45357</v>
+        <v>45408</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Champions League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Real Sociedad</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -3383,11 +3379,11 @@
         </is>
       </c>
       <c r="H60" t="n">
-        <v>38.5</v>
+        <v>37.82</v>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J60" t="inlineStr">
@@ -3399,56 +3395,56 @@
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>45361</v>
+        <v>45412</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Primera División</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Bayern München</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Celta</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>4-0</t>
+          <t>2-2</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H61" t="n">
-        <v>38.77</v>
+        <v>37.58</v>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>45367</v>
+        <v>45416</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -3457,32 +3453,30 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Osasuna</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Real Madrid</t>
+          <t>Cádiz</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>2-4</t>
+          <t>3-0</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="H62" t="n">
-        <v>40.14</v>
-      </c>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr"/>
       <c r="I62" t="inlineStr">
         <is>
           <t>Ganado</t>
@@ -3490,304 +3484,10 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K62" t="inlineStr"/>
-    </row>
-    <row r="63">
-      <c r="A63" s="2" t="n">
-        <v>45382</v>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>Primera División</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>Real Madrid</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>Athletic</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>2-0</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H63" t="n">
-        <v>38.48</v>
-      </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>Ganado</t>
-        </is>
-      </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K63" t="inlineStr"/>
-    </row>
-    <row r="64">
-      <c r="A64" s="2" t="n">
-        <v>45391</v>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>Champions League</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>Real Madrid</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>Manchester City</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>3-3</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H64" t="n">
-        <v>37.78</v>
-      </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>Empatado</t>
-        </is>
-      </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>NO SE REALIZA OPERACION</t>
-        </is>
-      </c>
-      <c r="K64" t="inlineStr"/>
-    </row>
-    <row r="65">
-      <c r="A65" s="2" t="n">
-        <v>45395</v>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>Primera División</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>Mallorca</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>Real Madrid</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>0-1</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H65" t="n">
-        <v>37.64</v>
-      </c>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>Ganado</t>
-        </is>
-      </c>
-      <c r="J65" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K65" t="inlineStr"/>
-    </row>
-    <row r="66">
-      <c r="A66" s="2" t="n">
-        <v>45399</v>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>Champions League</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Manchester City</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>Real Madrid</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>1 (3-4) 1</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="H66" t="n">
-        <v>38.66</v>
-      </c>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>Ganado</t>
-        </is>
-      </c>
-      <c r="J66" t="inlineStr">
-        <is>
-          <t>NO SE REALIZA OPERACION</t>
-        </is>
-      </c>
-      <c r="K66" t="inlineStr"/>
-    </row>
-    <row r="67">
-      <c r="A67" s="2" t="n">
-        <v>45403</v>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>Primera División</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>Real Madrid</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>Barcelona</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>3-2</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H67" t="n">
-        <v>38.46</v>
-      </c>
-      <c r="I67" t="inlineStr">
-        <is>
-          <t>Ganado</t>
-        </is>
-      </c>
-      <c r="J67" t="inlineStr">
-        <is>
-          <t>NO SE REALIZA OPERACION</t>
-        </is>
-      </c>
-      <c r="K67" t="inlineStr"/>
-    </row>
-    <row r="68">
-      <c r="A68" s="2" t="n">
-        <v>45408</v>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>Primera División</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>Real Sociedad</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>Real Madrid</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>0-1</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H68" t="n">
-        <v>37.82</v>
-      </c>
-      <c r="I68" t="inlineStr">
-        <is>
-          <t>Ganado</t>
-        </is>
-      </c>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>NO SE REALIZA OPERACION</t>
-        </is>
-      </c>
-      <c r="K68" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
cambios de 1 y -1 a compra y venta
</commit_message>
<xml_diff>
--- a/Futbol.xlsx
+++ b/Futbol.xlsx
@@ -538,7 +538,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K2" t="inlineStr"/>
@@ -636,7 +636,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K4" t="inlineStr"/>
@@ -685,7 +685,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>-1</t>
+          <t>Venta</t>
         </is>
       </c>
       <c r="K5" t="n">
@@ -785,7 +785,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K7" t="inlineStr"/>
@@ -834,7 +834,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K8" t="inlineStr"/>
@@ -932,7 +932,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K10" t="inlineStr"/>
@@ -981,7 +981,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K11" t="inlineStr"/>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>-1</t>
+          <t>Venta</t>
         </is>
       </c>
       <c r="K12" t="n">
@@ -1130,7 +1130,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K14" t="inlineStr"/>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K15" t="inlineStr"/>
@@ -1228,7 +1228,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K16" t="inlineStr"/>
@@ -1277,7 +1277,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K17" t="inlineStr"/>
@@ -1326,7 +1326,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K18" t="inlineStr"/>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K19" t="inlineStr"/>
@@ -1424,7 +1424,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>-1</t>
+          <t>Venta</t>
         </is>
       </c>
       <c r="K20" t="n">
@@ -1475,7 +1475,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K21" t="inlineStr"/>
@@ -1524,7 +1524,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K22" t="inlineStr"/>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K23" t="inlineStr"/>
@@ -1622,7 +1622,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K24" t="inlineStr"/>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K26" t="inlineStr"/>
@@ -1769,7 +1769,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K27" t="inlineStr"/>
@@ -1867,7 +1867,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K29" t="inlineStr"/>
@@ -1916,7 +1916,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K30" t="inlineStr"/>
@@ -1965,7 +1965,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K31" t="inlineStr"/>
@@ -2014,7 +2014,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
@@ -2504,7 +2504,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>-1</t>
+          <t>Venta</t>
         </is>
       </c>
       <c r="K42" t="n">
@@ -2555,7 +2555,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K43" t="inlineStr"/>
@@ -2604,7 +2604,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K44" t="inlineStr"/>
@@ -2653,7 +2653,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K45" t="inlineStr"/>
@@ -2751,7 +2751,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K47" t="inlineStr"/>
@@ -2800,7 +2800,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K48" t="inlineStr"/>
@@ -2898,7 +2898,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K50" t="inlineStr"/>
@@ -3045,7 +3045,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K53" t="inlineStr"/>
@@ -3094,7 +3094,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K54" t="inlineStr"/>
@@ -3143,7 +3143,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K55" t="inlineStr"/>
@@ -3241,7 +3241,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Compra</t>
         </is>
       </c>
       <c r="K57" t="inlineStr"/>

</xml_diff>